<commit_message>
Added Log4J framework and updated Excel reading method with Formatter
</commit_message>
<xml_diff>
--- a/NativeAppsAutomation/TestDataSheet.xlsx
+++ b/NativeAppsAutomation/TestDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097FE54D-39F1-4816-85F1-ACC3EBEE888A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C4C8EE-30BF-4FB8-974F-EE9A0EF39AEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Economy Class</t>
   </si>
   <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
     <t>March 2020</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>July 2020</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -170,9 +170,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +457,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +514,10 @@
       <c r="E2" s="4">
         <v>2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -528,25 +529,25 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -560,7 +561,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="A2:G3 C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +600,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -613,10 +614,10 @@
       <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>0</v>
       </c>
     </row>
@@ -625,21 +626,21 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -668,12 +669,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -686,7 +687,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,16 +718,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -742,7 +743,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,18 +781,18 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commiting from GitHub Desktop
</commit_message>
<xml_diff>
--- a/NativeAppsAutomation/TestDataSheet.xlsx
+++ b/NativeAppsAutomation/TestDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C4C8EE-30BF-4FB8-974F-EE9A0EF39AEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B296C24-94D0-4E66-BFF6-308D994151C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FlightBookingData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Month and Year</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Top 5 Luxury Beach Resorts in India</t>
-  </si>
-  <si>
-    <t>Dubai, 10 Incredible Things to do on Your First Visit</t>
   </si>
   <si>
     <t>February 2020</t>
@@ -529,7 +526,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>19</v>
@@ -560,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C5D303-5D75-425B-A301-066C2A3B0EB1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -600,7 +597,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -651,10 +648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C17D8F-7D6A-4336-9353-AE31183DF324}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,11 +667,6 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -718,16 +710,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -742,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD28E3D7-B65E-4E79-A0D5-FC7105B30604}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -781,7 +773,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>27</v>

</xml_diff>